<commit_message>
zg_quiz and homework for L1-L4
</commit_message>
<xml_diff>
--- a/porformance/zg_quiz.xlsx
+++ b/porformance/zg_quiz.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\roming vault\Log\life\jobs\南科大\传输现象助教\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\roming vault\Log\life\jobs\南科大\传输现象助教\transport phenomena\problems and solutions\porformance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="295">
   <si>
     <t>学生课堂考勤表</t>
   </si>
@@ -1163,6 +1163,90 @@
   </si>
   <si>
     <t>100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00</t>
+    </r>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2263,7 +2347,7 @@
   <dimension ref="A1:V133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -2467,7 +2551,9 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="5" t="s">
+        <v>292</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -2501,7 +2587,9 @@
       <c r="E6" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -2535,7 +2623,9 @@
       <c r="E7" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="5" t="s">
+        <v>292</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -2569,7 +2659,9 @@
       <c r="E8" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2601,7 +2693,9 @@
         <v>268</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -2635,7 +2729,9 @@
       <c r="E10" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -2669,7 +2765,9 @@
       <c r="E11" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2703,7 +2801,9 @@
       <c r="E12" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -2737,7 +2837,9 @@
       <c r="E13" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="5" t="s">
+        <v>294</v>
+      </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -2803,7 +2905,9 @@
         <v>271</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -2837,7 +2941,9 @@
       <c r="E16" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="5" t="s">
+        <v>293</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -2871,7 +2977,9 @@
       <c r="E17" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="5" t="s">
+        <v>294</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -2905,7 +3013,9 @@
       <c r="E18" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -2937,7 +3047,9 @@
         <v>267</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>289</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -2971,7 +3083,9 @@
       <c r="E20" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -3005,7 +3119,9 @@
       <c r="E21" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="F21" s="4"/>
+      <c r="F21" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -3039,7 +3155,9 @@
       <c r="E22" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="F22" s="4"/>
+      <c r="F22" s="5" t="s">
+        <v>292</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -3137,7 +3255,9 @@
       <c r="E25" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -3171,7 +3291,9 @@
       <c r="E26" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="F26" s="4"/>
+      <c r="F26" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -3205,7 +3327,9 @@
       <c r="E27" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -3239,7 +3363,9 @@
       <c r="E28" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="F28" s="4"/>
+      <c r="F28" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -3273,7 +3399,9 @@
       <c r="E29" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="F29" s="4"/>
+      <c r="F29" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -3307,7 +3435,9 @@
       <c r="E30" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -3341,7 +3471,9 @@
       <c r="E31" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="5" t="s">
+        <v>294</v>
+      </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -3407,7 +3539,9 @@
       <c r="E33" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="F33" s="4"/>
+      <c r="F33" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -3441,7 +3575,9 @@
       <c r="E34" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="F34" s="4"/>
+      <c r="F34" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -3475,7 +3611,9 @@
       <c r="E35" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="F35" s="4"/>
+      <c r="F35" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>

</xml_diff>